<commit_message>
added new files changes
</commit_message>
<xml_diff>
--- a/player_performance.xlsx
+++ b/player_performance.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,11 +468,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Faf du Plessis</t>
+          <t>MS Dhoni (WK)</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
@@ -481,32 +481,472 @@
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>179</v>
+        <v>28</v>
       </c>
       <c r="F2" t="n">
-        <v>278</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>Mustafizur Rahman</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>24</v>
+      </c>
+      <c r="F3" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
           <t>Virat Kohli</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>18</v>
+      </c>
+      <c r="F4" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Tushar Deshpande</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>23</v>
+      </c>
+      <c r="F5" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Deepak Chahar</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>17</v>
+      </c>
+      <c r="F6" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Cameron Green</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>2</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>16</v>
+      </c>
+      <c r="F7" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Ruturaj Gaikwad (C)</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>14</v>
+      </c>
+      <c r="F8" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Ravindra Jadeja</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>11</v>
+      </c>
+      <c r="F9" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Alzarri Josheph</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>2</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="n">
+        <v>13</v>
+      </c>
+      <c r="F10" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Faf du Plessis(C)</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="n">
+        <v>18</v>
+      </c>
+      <c r="F11" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Mayank Dagar</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>2</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" t="n">
+        <v>6</v>
+      </c>
+      <c r="F12" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Mohammed Siraj</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>2</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" t="n">
         <v>10</v>
       </c>
-      <c r="C3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" t="n">
-        <v>115</v>
-      </c>
-      <c r="F3" t="n">
-        <v>226</v>
+      <c r="F13" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Rachin Ravindra</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" t="n">
+        <v>7</v>
+      </c>
+      <c r="F14" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Dinesh Karthik</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" t="n">
+        <v>10</v>
+      </c>
+      <c r="F15" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Maheesh Theekshana</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" t="n">
+        <v>10</v>
+      </c>
+      <c r="F16" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Karn Sharma</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" t="n">
+        <v>4</v>
+      </c>
+      <c r="F17" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Anuj Rawat(WK)</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" t="n">
+        <v>13</v>
+      </c>
+      <c r="F18" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Sameer Rizvi</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" t="n">
+        <v>12</v>
+      </c>
+      <c r="F19" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Daryl Mitchell</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>0</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" t="n">
+        <v>2</v>
+      </c>
+      <c r="F20" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Ajinkya Rahane</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>0</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" t="n">
+        <v>8</v>
+      </c>
+      <c r="F21" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Glenn Maxwell</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" t="n">
+        <v>4</v>
+      </c>
+      <c r="F22" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Rajat Patidar</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>0</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" t="n">
+        <v>4</v>
+      </c>
+      <c r="F23" t="n">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>